<commit_message>
gui finished and integrated with bot.py
</commit_message>
<xml_diff>
--- a/Broward.xlsx
+++ b/Broward.xlsx
@@ -1,42 +1,220 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wesley\Desktop\cnadows\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B28E74-CCCF-4E95-83EE-D64B2EFAED3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12648" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>JOYCEMIN D AARONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7912 PEMBROKE ROAD
+MIRAMAR, FL 33023
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>SARAH  AARONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6225 SW 32nd st
+HOLLYWOOD, FL 33023
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>VALRETA M AARONS JONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brookd 4261 Spring Tree Drive
+FT LAUDERDALE, FL 33315
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>CARREN  AASER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5420 nw 33rd ave suite 100
+FORT LAUDERDALE, FL 33309
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>ZEETA DELORES ABABIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">620 NW 204TH AVENUE
+PEMBROKE PINES, FL 33029
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>RENELLE F ABACY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2617 NE 13th Ter
+Pompano Beach
+FL
+POMPANO BEACH, FL 33064
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>SAMARIA D ABARCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211 NE 8TH AVE
+APT 106
+HALLANDALE, FL 33009
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>NAGLAA A ABDELMAGED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4124 Inverarry Blvd
+Apt 61 A
+LAUDERHILL, FL 33319
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>BERNITE  ABDON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2941 Ne 1st Terrace
+WILTON MANOR, FL 33334
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>MI-CHELANGELINI C. FATIMA AKARKH ABDUKRAHMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320  S. FLAMINGO RD.
+PEMBROKE PINES, FL 33027
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>NADEZHDA B ABDURAKHMANOVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4800 NOB HILL RD.
+SUNRISE, FL 33323
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>NICOLE K ABEDRABBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404 sw 120 ave
+PEMBROKE PINES, FL 33025
+</t>
+  </si>
+  <si>
+    <t>MARIE C ABELARD</t>
+  </si>
+  <si>
+    <t>MARIE R ABELLARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1458 SW 116TH AVE
+PEMBROKE PINES, FL 33025
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>CAROLINE A ABIERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">375 SW 15th Street, #201
+POMPANO BEACH, FL 33060
+</t>
+  </si>
+  <si>
+    <t>KRYSTAL L ABNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">650  SW 28th Terr
+FORT LAUDERDALE, FL 33312
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>CLAUDIA  ABOUHANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401 NW 42ND AVE
+PLANTATION, FL 33317
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>SHERERONETTE S ABOY LAWSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4420 NW 59TH CT
+NORTH LAUDERDALE, FL 33319
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>ANEY  ABRAHAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">703 NORTH FLAMINGO ROAD
+PEMBROKE PINES, FL 33028
+UNITED STATES
+</t>
+  </si>
+  <si>
+    <t>JESEMIE  ABRAHAM SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2701 SW 88th Avenue
+MIRAMAR, FL 33025
+UNITED STATES
+</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,24 +230,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -335,15 +504,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B183"/>
+      <selection activeCell="A1" sqref="A1:B183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>